<commit_message>
Add dictionary configuration functionality
Implemented ability to manage constructed language dictionary words. A new section has been added, allowing admins to add, remove, and update words directly on the web page. The BuilderController has also been updated with relevant endpoint changes.
</commit_message>
<xml_diff>
--- a/EpochApp/Documents/ConfigWorksheet.xlsx
+++ b/EpochApp/Documents/ConfigWorksheet.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Projects\EpochWorlds\EpochApp\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3990C256-A2B3-4723-BAF0-79470288A06B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8EC7BF-9D19-4102-AB6C-5AF1CDC58403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8B44DA40-1F97-451E-9FB3-B049A21D1459}"/>
+    <workbookView xWindow="-24030" yWindow="1575" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{8B44DA40-1F97-451E-9FB3-B049A21D1459}"/>
   </bookViews>
   <sheets>
     <sheet name="lkMetaCategories" sheetId="1" r:id="rId1"/>
+    <sheet name="lkWordDict" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,6 +34,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Translation</t>
+  </si>
+  <si>
+    <t>PoS</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -383,10 +395,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8847C86-0338-490F-93E4-A5253FFE8531}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A44B5C7-A587-4396-982B-037A29240624}">
+  <dimension ref="B1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement tag service and enhance world metadata
A tag service has been implemented with new model classes for storing tags linked to users, articles and worlds. World metadata has been expanded to include more detailed properties like excerpts, headers, images and a collection of associated tags. Adjustments have also been made to the database context to accommodate these changes.
</commit_message>
<xml_diff>
--- a/EpochApp/Documents/ConfigWorksheet.xlsx
+++ b/EpochApp/Documents/ConfigWorksheet.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Projects\EpochWorlds\EpochApp\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8EC7BF-9D19-4102-AB6C-5AF1CDC58403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB11A57-1BD9-4A3C-9B7F-2FC8D183BE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24030" yWindow="1575" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{8B44DA40-1F97-451E-9FB3-B049A21D1459}"/>
+    <workbookView xWindow="-23370" yWindow="2310" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{8B44DA40-1F97-451E-9FB3-B049A21D1459}"/>
   </bookViews>
   <sheets>
     <sheet name="lkMetaCategories" sheetId="1" r:id="rId1"/>
-    <sheet name="lkWordDict" sheetId="2" r:id="rId2"/>
+    <sheet name="lkMetaTemplates" sheetId="3" r:id="rId2"/>
+    <sheet name="lkWordDict" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,24 +38,257 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="77">
   <si>
     <t>Translation</t>
   </si>
   <si>
     <t>PoS</t>
+  </si>
+  <si>
+    <t>Goals</t>
+  </si>
+  <si>
+    <t>Theme</t>
+  </si>
+  <si>
+    <t>Focus</t>
+  </si>
+  <si>
+    <t>Setting</t>
+  </si>
+  <si>
+    <t>Residents</t>
+  </si>
+  <si>
+    <t>Conflict</t>
+  </si>
+  <si>
+    <t>Inspiration</t>
+  </si>
+  <si>
+    <t>CategoryID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>TemplateID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Placeholder</t>
+  </si>
+  <si>
+    <t>HelpText</t>
+  </si>
+  <si>
+    <t>Motivation</t>
+  </si>
+  <si>
+    <t>What is the motivation for building the world?</t>
+  </si>
+  <si>
+    <t>I want to build an exciting world which indulges my passion for Age of Sail history in a D&amp;D context</t>
+  </si>
+  <si>
+    <t>Decide what the world is being built for, and what it means to you - that way, it’ll be fit for purpose!</t>
+  </si>
+  <si>
+    <t>Benefits</t>
+  </si>
+  <si>
+    <t>What is the benefit?</t>
+  </si>
+  <si>
+    <t>I am hoping to give my players an epic experience like "Black Sails" or "Master and Commander" with a DnD twist.</t>
+  </si>
+  <si>
+    <t>Knowing what you want from your worldbuilding project will help keep you on track when you get tired or stuck. Are you creating for a novel or a D&amp;D campaign? What kind of experience do you want your audience to have?</t>
+  </si>
+  <si>
+    <t>Hook</t>
+  </si>
+  <si>
+    <t>What makes your world different?</t>
+  </si>
+  <si>
+    <t>This is the core of your idea, the hook that draws you - and hopefully your players and readers - into the setting of the world. When we say “Unique” we really mean “special to you”. As long as you’re excited about the concept, that’s enough. Don’t feel like you have to reinvent the wheel and come up with something 100% original.</t>
+  </si>
+  <si>
+    <t>Instead of standard Medieval Fantasy, my world has newly discovered magic-powered airships. Exploration is now possible in a whole new way, and massive swathes of undiscovered territory cry out to be explored!</t>
+  </si>
+  <si>
+    <t>Genre</t>
+  </si>
+  <si>
+    <t>What is this world's genre?</t>
+  </si>
+  <si>
+    <t>Knowing the genre(s) and general technology/magic level will help you set expectations about your world, and keep your world feeling cohesive.</t>
+  </si>
+  <si>
+    <t>My world is Fantasy! Magi-punk fantasy with an Age of Sail (i.e. Renaissance) technology level fuelled by magic</t>
+  </si>
+  <si>
+    <t>Feel</t>
+  </si>
+  <si>
+    <t>How is the world experienced?</t>
+  </si>
+  <si>
+    <t>Do you want your world to feel mystical, or terrifying - or both? Should your audience be afraid or moved, filled with wanderlust or wonder? Awed by the past, or by the future? Your world will have a general feel to it, even if the specifics of tone vary from story to story.</t>
+  </si>
+  <si>
+    <t>World feels exciting and dangerous, and there are plenty of dark things there too - many of the newly discovered places are not very pleasant. But it's an epic campaign setting.</t>
+  </si>
+  <si>
+    <t>Tone</t>
+  </si>
+  <si>
+    <t>What is the tone?</t>
+  </si>
+  <si>
+    <t>World is Darkish - think Witcher rather than Dark Souls.</t>
+  </si>
+  <si>
+    <t>PrimaryFocus</t>
+  </si>
+  <si>
+    <t>SecondaryFocus</t>
+  </si>
+  <si>
+    <t>TertiaryFocus</t>
+  </si>
+  <si>
+    <t>AncillaryFocus</t>
+  </si>
+  <si>
+    <t>Choose three to five focal points of your world to focus your worldbuilding on</t>
+  </si>
+  <si>
+    <t>Military: there is a cold war between different countries, all eager for this new kind of technology and looking for ways to weaponise it. Think espionage and kidnapping of scientists and mages.</t>
+  </si>
+  <si>
+    <t>Technology: now the initial ships have been invented, there is a surge in new models, techniques and improvements to the original technology. Everybody is looking for new ways to use and improve the Airships. There is also a "space race" between the different nations, all trying to adopt this technology.</t>
+  </si>
+  <si>
+    <t>Gender Relations: this has always been a man's world, but the magic type required to fly the airships is only operable by women, and not men. Suddenly, women are being percieved in a whole new way.</t>
+  </si>
+  <si>
+    <t>Primary Focus</t>
+  </si>
+  <si>
+    <t>Secondary Focus</t>
+  </si>
+  <si>
+    <t>Tertiary Focus</t>
+  </si>
+  <si>
+    <t>Ancillary Focus</t>
+  </si>
+  <si>
+    <t>PrimaryDifferences</t>
+  </si>
+  <si>
+    <t>What are the primary differences between reality and your world?</t>
+  </si>
+  <si>
+    <t>Does your world have magic or altered gravity, midichlorians or psionics? Are the gods wandering the world? Nail down your world’s natural laws now - they will have fundamental repercussions on everything else in your world!</t>
+  </si>
+  <si>
+    <t>1. There is magic.
+2. The magic is the energy generated by your dreams and refreshed during your sleep. It can be harnessed during your waking hours.
+3. Magic is expressed differently based on your genetic predispositions, gender and species.</t>
+  </si>
+  <si>
+    <t>Cosmology</t>
+  </si>
+  <si>
+    <t>What is this world's origin?</t>
+  </si>
+  <si>
+    <t>The dominant religion, The Children of the Suns, believes that the world is the child of the twin suns, La and Tho. In reality, the world was intentionally created from a nebula by aliens who will be back to check on it someday…</t>
+  </si>
+  <si>
+    <t>Nobody knows, but the dominant religion, The Children of the Suns, believes that the world is the child of the twin suns, La and Tho…</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Summarize a brief history of those who live in your world…</t>
+  </si>
+  <si>
+    <t>Inhabitants</t>
+  </si>
+  <si>
+    <t>Who or what are the inhabitants of your world?</t>
+  </si>
+  <si>
+    <t>The old world is inhabited by 5 human empires living, until recently at least, in relative peace. A kingdom of dragon-riding dwarves dominates the northern mountain ranges. The western wildlands are inhabited by the nomadic orc-clans of Torg-'Xhai.</t>
+  </si>
+  <si>
+    <t>PrimaryDrama</t>
+  </si>
+  <si>
+    <t>SecondaryDrama</t>
+  </si>
+  <si>
+    <t>TertiaryDrama</t>
+  </si>
+  <si>
+    <t>AncillaryDrama</t>
+  </si>
+  <si>
+    <t>Primary Drama</t>
+  </si>
+  <si>
+    <t>Secondary Drama</t>
+  </si>
+  <si>
+    <t>Tertiary Drama</t>
+  </si>
+  <si>
+    <t>Ancillary Drama</t>
+  </si>
+  <si>
+    <t>Imagery</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Literature</t>
+  </si>
+  <si>
+    <t>Games</t>
+  </si>
+  <si>
+    <t>Movies</t>
+  </si>
+  <si>
+    <t>Shows</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Space Mono"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Space Mono"/>
     </font>
   </fonts>
   <fills count="2">
@@ -77,8 +311,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,21 +631,461 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8847C86-0338-490F-93E4-A5253FFE8531}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF56751-B997-40F5-AAF7-26D034645785}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.88671875" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="90">
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A44B5C7-A587-4396-982B-037A29240624}">
   <dimension ref="B1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>